<commit_message>
minor UI bugs related to map and charts are fixed
</commit_message>
<xml_diff>
--- a/public/data/TABAQAT.xlsx
+++ b/public/data/TABAQAT.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\informatic iran\OneDrive\Desktop\New folder\2chnar 12\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Hominex\mahallat\public\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8A192A7-F406-4492-BF68-07A5494480A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B289779B-F02F-4FB7-80BB-A171C3C73901}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4728" yWindow="1632" windowWidth="17280" windowHeight="8880" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="768" yWindow="768" windowWidth="17280" windowHeight="8880" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="3c316ed6-8cae-4cac-8b34-e2df2df" sheetId="1" r:id="rId1"/>
@@ -30,9 +30,6 @@
     <t>تعداد</t>
   </si>
   <si>
-    <t>همکف و ویلایی</t>
-  </si>
-  <si>
     <t>یک طبقه</t>
   </si>
   <si>
@@ -58,6 +55,9 @@
   </si>
   <si>
     <t>طبقات</t>
+  </si>
+  <si>
+    <t>همکف</t>
   </si>
 </sst>
 </file>
@@ -228,7 +228,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C9"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J7" sqref="J7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
@@ -239,13 +241,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -256,7 +258,7 @@
         <v>490</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -267,7 +269,7 @@
         <v>196</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -278,7 +280,7 @@
         <v>166</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -289,7 +291,7 @@
         <v>150</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -300,7 +302,7 @@
         <v>39</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -311,7 +313,7 @@
         <v>29</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -322,7 +324,7 @@
         <v>5</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -333,7 +335,7 @@
         <v>51</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>